<commit_message>
finished dynamic excel reading
</commit_message>
<xml_diff>
--- a/Test Documents/testmsheetoffsetcol.xlsx
+++ b/Test Documents/testmsheetoffsetcol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Statistical-Performance-Measures\Test Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6517D5B8-BBBB-4A18-8310-E582D5ED3112}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{984AB455-408A-4B4E-B64D-91A98B03C1ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{9218FA83-5AFF-4FD3-A0D8-B584414673FF}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{9218FA83-5AFF-4FD3-A0D8-B584414673FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -455,7 +455,7 @@
   <dimension ref="D1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:T4"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,7 +748,7 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,7 +812,7 @@
         <v>40728.569447222224</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G2">
         <f>SUM(B2:B4)/3</f>
@@ -820,39 +820,39 @@
       </c>
       <c r="H2">
         <f>SUM(E2:E4)/3</f>
-        <v>5.3333333333333337E-2</v>
+        <v>0.12666666666666668</v>
       </c>
       <c r="I2">
         <f>((B2-G2)*(E2-H2)+(B3-G2)*(E3-H2)+(B4-G2)*(E4-H2))/(SQRT((B2-G2)^2+(B3-G2)^2+(B4-G2)^2)*SQRT((E2-H2)^2+(E3-H2)^2+(E4-H2)^2))</f>
-        <v>0.49999999999999994</v>
+        <v>0.7559289460184544</v>
       </c>
       <c r="J2">
         <f>I2^2</f>
-        <v>0.24999999999999994</v>
+        <v>0.57142857142857129</v>
       </c>
       <c r="K2" s="6">
         <f>1-(((B2-E2)^2+(B3-E3)^2+(B4-E4)^2)/((B2-G2)^2+(B3-G2)^2+(B4-G2)^2))</f>
-        <v>-349.2270886409479</v>
+        <v>-577.39288862780859</v>
       </c>
       <c r="L2">
         <f>1-(((B2-E2)^2+(B3-E3)^2+(B4-E4)^2)/((ABS(E2-G2)+ABS(B2-G2))^2+(ABS(E3-G2)+ABS(B3-G2))^2+(ABS(E4-G2)+ABS(B4-G2))^2))</f>
-        <v>0.11062320421949146</v>
+        <v>8.0041348436912685E-2</v>
       </c>
       <c r="M2">
         <f>SQRT((1/3)*((B2-E2)^2+(B3-E3)^2+(B4-E4)^2))</f>
-        <v>7.7021535879190306E-2</v>
+        <v>9.8980303226910593E-2</v>
       </c>
       <c r="N2">
         <f>(1/3)*(ABS(B2-E2)+ABS(B3-E3)+ABS(B4-E4))</f>
-        <v>6.1447203202682696E-2</v>
+        <v>9.6504664115969863E-2</v>
       </c>
       <c r="O2">
         <f>(SQRT(((B2-E2)^2+(B3-E3)^2+(B4-E4)^2)))/SQRT((B2-H2)^2+(B3-H2)^2+(B4-H2)^2)</f>
-        <v>3.2727773751228959</v>
+        <v>1.0247216078047181</v>
       </c>
       <c r="Q2">
         <f>(((B2-E2)+(B3-E3)+(B4-E4))/SUM(B2:B4))*100</f>
-        <v>-76.822918981224021</v>
+        <v>-319.95443258040706</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -866,7 +866,7 @@
         <v>40728.570836168983</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>